<commit_message>
update modules/ticket: mod        5 files
</commit_message>
<xml_diff>
--- a/starter/src/main/resources/excel/team_member.xlsx
+++ b/starter/src/main/resources/excel/team_member.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30440" windowHeight="12040"/>
+    <workbookView windowWidth="26980" windowHeight="11380"/>
   </bookViews>
   <sheets>
     <sheet name="自动回复" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Nickname</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>102@email.com</t>
+  </si>
+  <si>
+    <t>member</t>
   </si>
   <si>
     <t>test3</t>
@@ -707,7 +710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1094,7 +1097,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1190,6 +1193,9 @@
       <c r="D4">
         <v>2</v>
       </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
       <c r="F4">
         <v>2</v>
       </c>
@@ -1199,16 +1205,19 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>18800000003</v>
       </c>
       <c r="D5">
         <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -1219,16 +1228,19 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>18800000004</v>
       </c>
       <c r="D6">
         <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -1239,16 +1251,19 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>18800000005</v>
       </c>
       <c r="D7">
         <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
       </c>
       <c r="F7">
         <v>5</v>

</xml_diff>